<commit_message>
New results using directly google API
</commit_message>
<xml_diff>
--- a/results/maps_on_reasoning_models/summary_results.xlsx
+++ b/results/maps_on_reasoning_models/summary_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -553,7 +553,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>google/gemini-2.5-flash-preview-05-20</t>
+          <t>gemini-2.5-flash-preview-05-20</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -566,22 +566,22 @@
         <v>30</v>
       </c>
       <c r="G2" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="L2" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="M2" t="n">
         <v>30</v>
@@ -593,22 +593,22 @@
         <v>0.6666666666666666</v>
       </c>
       <c r="P2" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.03333333333333333</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="R2" t="n">
-        <v>0</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="S2" t="n">
         <v>0</v>
       </c>
       <c r="T2" t="n">
-        <v>0.7</v>
+        <v>0.7333333333333333</v>
       </c>
       <c r="U2" t="n">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3">
@@ -624,32 +624,32 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>o4-mini-2025-04-16</t>
+          <t>gemini-2.5-pro-preview-05-06</t>
         </is>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="F3" t="n">
         <v>30</v>
       </c>
       <c r="G3" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H3" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="L3" t="n">
         <v>27</v>
@@ -661,25 +661,96 @@
         <v>0</v>
       </c>
       <c r="O3" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.9</v>
       </c>
       <c r="P3" t="n">
-        <v>0.7666666666666667</v>
+        <v>0.9</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="R3" t="n">
-        <v>0.06666666666666667</v>
+        <v>0</v>
       </c>
       <c r="S3" t="n">
-        <v>0.06666666666666667</v>
+        <v>0</v>
       </c>
       <c r="T3" t="n">
-        <v>0.7666666666666667</v>
+        <v>0.9</v>
       </c>
       <c r="U3" t="n">
         <v>0.9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AIME</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>AIME</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>o4-mini-2025-04-16</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24</v>
+      </c>
+      <c r="F4" t="n">
+        <v>30</v>
+      </c>
+      <c r="G4" t="n">
+        <v>26</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>25</v>
+      </c>
+      <c r="L4" t="n">
+        <v>26</v>
+      </c>
+      <c r="M4" t="n">
+        <v>30</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.03333333333333333</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.8666666666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add config to use the same auto prompt for all layers
</commit_message>
<xml_diff>
--- a/results/maps_on_reasoning_models/summary_results.xlsx
+++ b/results/maps_on_reasoning_models/summary_results.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB698ECD-962B-487C-AB0F-F57A56B000F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E9792B-A01E-47F9-AFF2-A0C09FEFD1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>dataset</t>
   </si>
@@ -98,6 +98,12 @@
   </si>
   <si>
     <t>MATH</t>
+  </si>
+  <si>
+    <t>gsm8-std</t>
+  </si>
+  <si>
+    <t>GSM8K</t>
   </si>
 </sst>
 </file>
@@ -153,11 +159,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -461,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U7"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -733,198 +740,328 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
         <v>84</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="3">
         <v>100</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="3">
         <v>86</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="3">
         <v>2</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="3">
         <v>1</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="3">
         <v>1</v>
       </c>
-      <c r="K5" s="2">
+      <c r="K5" s="3">
         <v>86</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="3">
         <v>88</v>
       </c>
-      <c r="M5" s="2">
+      <c r="M5" s="3">
         <v>100</v>
       </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
+      <c r="N5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
         <v>0.84</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="3">
         <v>0.86</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="3">
         <v>0.02</v>
       </c>
-      <c r="R5" s="2">
+      <c r="R5" s="3">
         <v>0.01</v>
       </c>
-      <c r="S5" s="2">
+      <c r="S5" s="3">
         <v>0.01</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="3">
         <v>0.86</v>
       </c>
-      <c r="U5" s="2">
+      <c r="U5" s="3">
         <v>0.88</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>84</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6">
         <v>100</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6">
         <v>86</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6">
         <v>1</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6">
         <v>1</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6">
         <v>86</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6">
         <v>88</v>
       </c>
-      <c r="M6" s="2">
+      <c r="M6">
         <v>100</v>
       </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
         <v>0.84</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6">
         <v>0.86</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6">
         <v>0.02</v>
       </c>
-      <c r="R6" s="2">
+      <c r="R6">
         <v>0.01</v>
       </c>
-      <c r="S6" s="2">
+      <c r="S6">
         <v>0.01</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6">
         <v>0.86</v>
       </c>
-      <c r="U6" s="2">
+      <c r="U6">
         <v>0.88</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>76</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7">
         <v>100</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7">
         <v>82</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7">
         <v>5</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7">
         <v>1</v>
       </c>
-      <c r="J7" s="2">
-        <v>0</v>
-      </c>
-      <c r="K7" s="2">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>81</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7">
         <v>82</v>
       </c>
-      <c r="M7" s="2">
+      <c r="M7">
         <v>100</v>
       </c>
-      <c r="N7" s="2">
-        <v>0</v>
-      </c>
-      <c r="O7" s="2">
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
         <v>0.76</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7">
         <v>0.82</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7">
         <v>0.05</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7">
         <v>0.01</v>
       </c>
-      <c r="S7" s="2">
-        <v>0</v>
-      </c>
-      <c r="T7" s="2">
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
         <v>0.81</v>
       </c>
-      <c r="U7" s="2">
+      <c r="U7">
         <v>0.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2">
+        <v>96</v>
+      </c>
+      <c r="F8" s="2">
+        <v>100</v>
+      </c>
+      <c r="G8" s="2">
+        <v>98</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0</v>
+      </c>
+      <c r="K8" s="2">
+        <v>97</v>
+      </c>
+      <c r="L8" s="2">
+        <v>98</v>
+      </c>
+      <c r="M8" s="2">
+        <v>100</v>
+      </c>
+      <c r="N8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="P8" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="R8" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0</v>
+      </c>
+      <c r="T8" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="U8" s="2">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>96</v>
+      </c>
+      <c r="F9" s="2">
+        <v>100</v>
+      </c>
+      <c r="G9" s="2">
+        <v>97</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>98</v>
+      </c>
+      <c r="L9" s="2">
+        <v>99</v>
+      </c>
+      <c r="M9" s="2">
+        <v>100</v>
+      </c>
+      <c r="N9" s="2">
+        <v>0</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0.96</v>
+      </c>
+      <c r="P9" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="R9" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0</v>
+      </c>
+      <c r="T9" s="2">
+        <v>0.98</v>
+      </c>
+      <c r="U9" s="2">
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add results for gemini 2.5 pro. Adjust config to run all benchs
</commit_message>
<xml_diff>
--- a/results/maps_on_reasoning_models/summary_results.xlsx
+++ b/results/maps_on_reasoning_models/summary_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E9792B-A01E-47F9-AFF2-A0C09FEFD1F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F179D46-EE1A-4CC8-9C1F-BA22FC2C6931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -159,12 +159,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -470,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,68 +609,68 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>27</v>
-      </c>
-      <c r="F3">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>24</v>
+      </c>
+      <c r="F3" s="2">
         <v>30</v>
       </c>
-      <c r="G3">
-        <v>27</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <v>27</v>
-      </c>
-      <c r="L3">
-        <v>27</v>
-      </c>
-      <c r="M3">
+      <c r="G3" s="2">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2">
+        <v>24</v>
+      </c>
+      <c r="L3" s="2">
+        <v>26</v>
+      </c>
+      <c r="M3" s="2">
         <v>30</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0.9</v>
-      </c>
-      <c r="P3">
-        <v>0.9</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0.9</v>
-      </c>
-      <c r="U3">
-        <v>0.9</v>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="S3" s="2">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0.8666666666666667</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -740,67 +739,67 @@
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
         <v>84</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>100</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>86</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3">
-        <v>1</v>
-      </c>
-      <c r="K5" s="3">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
         <v>86</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5">
         <v>88</v>
       </c>
-      <c r="M5" s="3">
+      <c r="M5">
         <v>100</v>
       </c>
-      <c r="N5" s="3">
-        <v>0</v>
-      </c>
-      <c r="O5" s="3">
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>0.84</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5">
         <v>0.86</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="Q5">
         <v>0.02</v>
       </c>
-      <c r="R5" s="3">
+      <c r="R5">
         <v>0.01</v>
       </c>
-      <c r="S5" s="3">
+      <c r="S5">
         <v>0.01</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5">
         <v>0.86</v>
       </c>
-      <c r="U5" s="3">
+      <c r="U5">
         <v>0.88</v>
       </c>
     </row>
@@ -935,132 +934,132 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>96</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8">
         <v>100</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8">
         <v>98</v>
       </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <v>0</v>
-      </c>
-      <c r="K8" s="2">
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
         <v>97</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8">
         <v>98</v>
       </c>
-      <c r="M8" s="2">
+      <c r="M8">
         <v>100</v>
       </c>
-      <c r="N8" s="2">
-        <v>0</v>
-      </c>
-      <c r="O8" s="2">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
         <v>0.96</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8">
         <v>0.98</v>
       </c>
-      <c r="Q8" s="2">
+      <c r="Q8">
         <v>0.01</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8">
         <v>0.01</v>
       </c>
-      <c r="S8" s="2">
-        <v>0</v>
-      </c>
-      <c r="T8" s="2">
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
         <v>0.97</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8">
         <v>0.98</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
         <v>96</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9">
         <v>100</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9">
         <v>97</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9">
         <v>2</v>
       </c>
-      <c r="I9" s="2">
-        <v>1</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0</v>
-      </c>
-      <c r="K9" s="2">
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
         <v>98</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9">
         <v>99</v>
       </c>
-      <c r="M9" s="2">
+      <c r="M9">
         <v>100</v>
       </c>
-      <c r="N9" s="2">
-        <v>0</v>
-      </c>
-      <c r="O9" s="2">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>0.96</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9">
         <v>0.97</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9">
         <v>0.02</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9">
         <v>0.01</v>
       </c>
-      <c r="S9" s="2">
-        <v>0</v>
-      </c>
-      <c r="T9" s="2">
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
         <v>0.98</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9">
         <v>0.99</v>
       </c>
     </row>

</xml_diff>